<commit_message>
Fixed bug in generate_slices calculating hi values in df.
</commit_message>
<xml_diff>
--- a/slices_dam.xlsx
+++ b/slices_dam.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/CursorProjects/slopetools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5986A0E-C163-254A-872C-5281EB24D717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEA6AE27-FFD0-6C49-9953-C204848D92C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18360" yWindow="2740" windowWidth="47240" windowHeight="19720" xr2:uid="{A0AD1E59-D55E-174B-B2C6-A92686281A3C}"/>
+    <workbookView xWindow="4880" yWindow="1820" windowWidth="58660" windowHeight="22160" xr2:uid="{DC92B59B-CC2B-514A-AB7B-2658B60DC874}"/>
   </bookViews>
   <sheets>
     <sheet name="slices" sheetId="1" r:id="rId1"/>
@@ -152,7 +152,7 @@
   <numFmts count="1">
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -285,6 +285,13 @@
       <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -629,18 +636,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1017,206 +1021,207 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F0FD57-722B-3C42-8681-C78F5F932DFD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7416AFE-B480-6642-8B00-FC9A7D5C328C}">
   <dimension ref="A1:AO23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="15" width="10.83203125" style="1"/>
-    <col min="16" max="18" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="33" width="10.83203125" style="1"/>
-    <col min="34" max="34" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="18" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="41" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:41" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="1">
         <v>-31.371763938475599</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="1">
         <v>226.96069945941201</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="1">
         <v>227</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="1">
         <v>-15.6858819692378</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="1">
         <v>219.95397393821199</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="1">
         <v>227</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="1">
         <v>-23.5288229538567</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="1">
         <v>223.32396218747999</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="1">
         <v>227</v>
       </c>
-      <c r="K2" s="4">
-        <v>225.16198109374</v>
-      </c>
-      <c r="L2" s="4">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1">
         <v>15.6858819692378</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="1">
         <v>-24.059548355183399</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="1">
         <v>17.1782937000103</v>
       </c>
       <c r="O2" s="1">
         <v>0</v>
       </c>
-      <c r="P2" s="3">
-        <v>3.6760378125194899</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>0</v>
-      </c>
-      <c r="R2" s="3">
-        <v>0</v>
-      </c>
-      <c r="S2" s="3">
-        <v>7092.4131147212302</v>
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
       </c>
       <c r="T2" s="1">
         <v>4680</v>
@@ -1224,13 +1229,13 @@
       <c r="U2" s="1">
         <v>4680</v>
       </c>
-      <c r="V2" s="3">
+      <c r="V2" s="1">
         <v>73409.927616033005</v>
       </c>
-      <c r="W2" s="3">
+      <c r="W2" s="1">
         <v>-23.5288229538567</v>
       </c>
-      <c r="X2" s="3">
+      <c r="X2" s="1">
         <v>227</v>
       </c>
       <c r="Y2" s="1">
@@ -1242,7 +1247,7 @@
       <c r="AA2" s="1">
         <v>0</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AB2" s="1">
         <v>0</v>
       </c>
       <c r="AC2" s="1">
@@ -1260,17 +1265,15 @@
       <c r="AG2" s="1">
         <v>302</v>
       </c>
-      <c r="AH2" s="3">
+      <c r="AH2" s="1">
         <v>78.676037812519496</v>
       </c>
-      <c r="AI2" s="3">
+      <c r="AI2" s="1">
         <v>4909.3847595012103</v>
       </c>
-      <c r="AJ2" s="1">
-        <v>2</v>
-      </c>
+      <c r="AJ2" s="1"/>
       <c r="AK2" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AL2" s="1">
         <v>0</v>
@@ -1286,62 +1289,60 @@
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="1">
         <v>-15.6858819692378</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="1">
         <v>219.95397393821199</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="1">
         <v>227</v>
       </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4">
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
         <v>213.97727363022301</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="1">
         <v>227</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="1">
         <v>-7.8429409846189104</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="1">
         <v>216.84121048466801</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="1">
         <v>227</v>
       </c>
-      <c r="K3" s="4">
-        <v>221.92060524233401</v>
-      </c>
-      <c r="L3" s="4">
+      <c r="K3" s="1"/>
+      <c r="L3" s="1">
         <v>15.6858819692378</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="1">
         <v>-20.849673877257999</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="1">
         <v>16.785006904582499</v>
       </c>
       <c r="O3" s="1">
         <v>0</v>
       </c>
-      <c r="P3" s="3">
-        <v>10.158789515331801</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>0</v>
-      </c>
-      <c r="R3" s="3">
-        <v>0</v>
-      </c>
-      <c r="S3" s="3">
-        <v>19599.997514402501</v>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
       </c>
       <c r="T3" s="1">
         <v>4680</v>
@@ -1349,13 +1350,13 @@
       <c r="U3" s="1">
         <v>4680</v>
       </c>
-      <c r="V3" s="3">
+      <c r="V3" s="1">
         <v>73409.927616033005</v>
       </c>
-      <c r="W3" s="3">
+      <c r="W3" s="1">
         <v>-7.8429409846189104</v>
       </c>
-      <c r="X3" s="3">
+      <c r="X3" s="1">
         <v>227</v>
       </c>
       <c r="Y3" s="1">
@@ -1367,7 +1368,7 @@
       <c r="AA3" s="1">
         <v>0</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="AB3" s="1">
         <v>0</v>
       </c>
       <c r="AC3" s="1">
@@ -1385,17 +1386,15 @@
       <c r="AG3" s="1">
         <v>302</v>
       </c>
-      <c r="AH3" s="3">
+      <c r="AH3" s="1">
         <v>85.158789515331804</v>
       </c>
-      <c r="AI3" s="3">
+      <c r="AI3" s="1">
         <v>5313.9084657567</v>
       </c>
-      <c r="AJ3" s="1">
-        <v>2</v>
-      </c>
+      <c r="AJ3" s="1"/>
       <c r="AK3" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AL3" s="1">
         <v>0</v>
@@ -1411,62 +1410,60 @@
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
         <v>213.97727363022301</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="1">
         <v>227</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="1">
         <v>18.75</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="1">
         <v>208.096869663924</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="1">
         <v>233.25</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="1">
         <v>9.375</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="1">
         <v>210.87008218622501</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="1">
         <v>230.125</v>
       </c>
-      <c r="K4" s="4">
-        <v>220.51876820056</v>
-      </c>
-      <c r="L4" s="4">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1">
         <v>18.75</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="1">
         <v>-17.4030992934183</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="1">
         <v>19.649471224888298</v>
       </c>
       <c r="O4" s="1">
         <v>0</v>
       </c>
-      <c r="P4" s="3">
-        <v>16.129917813774501</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>0</v>
-      </c>
-      <c r="R4" s="3">
-        <v>3.125</v>
-      </c>
-      <c r="S4" s="3">
-        <v>44523.841708017397</v>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
       </c>
       <c r="T4" s="1">
         <v>4680</v>
@@ -1474,13 +1471,13 @@
       <c r="U4" s="1">
         <v>4290</v>
       </c>
-      <c r="V4" s="3">
+      <c r="V4" s="1">
         <v>84093.75</v>
       </c>
-      <c r="W4" s="3">
+      <c r="W4" s="1">
         <v>9.2391304347826093</v>
       </c>
-      <c r="X4" s="3">
+      <c r="X4" s="1">
         <v>230.07971014492699</v>
       </c>
       <c r="Y4" s="1">
@@ -1492,7 +1489,7 @@
       <c r="AA4" s="1">
         <v>0</v>
       </c>
-      <c r="AB4" s="2">
+      <c r="AB4" s="1">
         <v>18.434948822921999</v>
       </c>
       <c r="AC4" s="1">
@@ -1510,17 +1507,15 @@
       <c r="AG4" s="1">
         <v>302</v>
       </c>
-      <c r="AH4" s="3">
+      <c r="AH4" s="1">
         <v>91.129917813774497</v>
       </c>
-      <c r="AI4" s="3">
+      <c r="AI4" s="1">
         <v>5686.5068715795296</v>
       </c>
-      <c r="AJ4" s="1">
-        <v>2</v>
-      </c>
+      <c r="AJ4" s="1"/>
       <c r="AK4" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AL4" s="1">
         <v>0</v>
@@ -1536,62 +1531,60 @@
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="1">
         <v>18.75</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="1">
         <v>208.096869663924</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="1">
         <v>233.25</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="1">
         <v>37.5</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="1">
         <v>203.51602066890601</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="1">
         <v>239.5</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="1">
         <v>28.125</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="1">
         <v>205.64819624299901</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="1">
         <v>236.375</v>
       </c>
-      <c r="K5" s="4">
-        <v>221.06430097041201</v>
-      </c>
-      <c r="L5" s="4">
+      <c r="K5" s="1"/>
+      <c r="L5" s="1">
         <v>18.75</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="1">
         <v>-13.722002629195799</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="1">
         <v>19.300883934393699</v>
       </c>
       <c r="O5" s="1">
         <v>0</v>
       </c>
-      <c r="P5" s="3">
-        <v>21.351803757000901</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>0</v>
-      </c>
-      <c r="R5" s="3">
-        <v>9.375</v>
-      </c>
-      <c r="S5" s="3">
-        <v>71215.253664583404</v>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
       </c>
       <c r="T5" s="1">
         <v>4290</v>
@@ -1599,13 +1592,13 @@
       <c r="U5" s="1">
         <v>3900</v>
       </c>
-      <c r="V5" s="3">
+      <c r="V5" s="1">
         <v>76781.25</v>
       </c>
-      <c r="W5" s="3">
+      <c r="W5" s="1">
         <v>27.9761904761904</v>
       </c>
-      <c r="X5" s="3">
+      <c r="X5" s="1">
         <v>236.32539682539601</v>
       </c>
       <c r="Y5" s="1">
@@ -1617,7 +1610,7 @@
       <c r="AA5" s="1">
         <v>0</v>
       </c>
-      <c r="AB5" s="2">
+      <c r="AB5" s="1">
         <v>18.434948822921999</v>
       </c>
       <c r="AC5" s="1">
@@ -1635,17 +1628,15 @@
       <c r="AG5" s="1">
         <v>302</v>
       </c>
-      <c r="AH5" s="3">
+      <c r="AH5" s="1">
         <v>96.351803757000894</v>
       </c>
-      <c r="AI5" s="3">
+      <c r="AI5" s="1">
         <v>6012.3525544368504</v>
       </c>
-      <c r="AJ5" s="1">
-        <v>2</v>
-      </c>
+      <c r="AJ5" s="1"/>
       <c r="AK5" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AL5" s="1">
         <v>0</v>
@@ -1661,62 +1652,60 @@
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="1">
         <v>37.5</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="1">
         <v>203.51602066890601</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="1">
         <v>239.5</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="1">
         <v>56.25</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="1">
         <v>200.175155298964</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="1">
         <v>245.75</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="1">
         <v>46.875</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="1">
         <v>201.69355626302601</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="1">
         <v>242.625</v>
       </c>
-      <c r="K6" s="4">
-        <v>222.23733328789601</v>
-      </c>
-      <c r="L6" s="4">
+      <c r="K6" s="1"/>
+      <c r="L6" s="1">
         <v>18.75</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="1">
         <v>-10.0978645610996</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="1">
         <v>19.045012668625201</v>
       </c>
       <c r="O6" s="1">
         <v>0</v>
       </c>
-      <c r="P6" s="3">
-        <v>25.3064437369732</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>0</v>
-      </c>
-      <c r="R6" s="3">
-        <v>15.625</v>
-      </c>
-      <c r="S6" s="3">
-        <v>94984.079618394593</v>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
       </c>
       <c r="T6" s="1">
         <v>3900</v>
@@ -1724,13 +1713,13 @@
       <c r="U6" s="1">
         <v>3510</v>
       </c>
-      <c r="V6" s="3">
+      <c r="V6" s="1">
         <v>69468.75</v>
       </c>
-      <c r="W6" s="3">
+      <c r="W6" s="1">
         <v>46.710526315789402</v>
       </c>
-      <c r="X6" s="3">
+      <c r="X6" s="1">
         <v>242.57017543859601</v>
       </c>
       <c r="Y6" s="1">
@@ -1742,7 +1731,7 @@
       <c r="AA6" s="1">
         <v>0</v>
       </c>
-      <c r="AB6" s="2">
+      <c r="AB6" s="1">
         <v>18.434948822921999</v>
       </c>
       <c r="AC6" s="1">
@@ -1760,17 +1749,15 @@
       <c r="AG6" s="1">
         <v>302</v>
       </c>
-      <c r="AH6" s="3">
+      <c r="AH6" s="1">
         <v>100.30644373697299</v>
       </c>
-      <c r="AI6" s="3">
+      <c r="AI6" s="1">
         <v>6259.1220891871299</v>
       </c>
-      <c r="AJ6" s="1">
-        <v>2</v>
-      </c>
+      <c r="AJ6" s="1"/>
       <c r="AK6" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AL6" s="1">
         <v>0</v>
@@ -1786,62 +1773,60 @@
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="1">
         <v>56.25</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="1">
         <v>200.175155298964</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="1">
         <v>245.75</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="1">
         <v>75</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="1">
         <v>198.033114398283</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="1">
         <v>252</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="1">
         <v>65.625</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="1">
         <v>198.95621684711699</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="1">
         <v>248.875</v>
       </c>
-      <c r="K7" s="4">
-        <v>224.014813069914</v>
-      </c>
-      <c r="L7" s="4">
+      <c r="K7" s="1"/>
+      <c r="L7" s="1">
         <v>18.75</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="1">
         <v>-6.5141648820616203</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="1">
         <v>18.871839639201902</v>
       </c>
       <c r="O7" s="1">
         <v>0</v>
       </c>
-      <c r="P7" s="3">
-        <v>28.043783152882899</v>
-      </c>
-      <c r="Q7" s="3">
-        <v>0</v>
-      </c>
-      <c r="R7" s="3">
-        <v>21.875</v>
-      </c>
-      <c r="S7" s="3">
-        <v>115945.506146336</v>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
       </c>
       <c r="T7" s="1">
         <v>3510</v>
@@ -1849,13 +1834,13 @@
       <c r="U7" s="1">
         <v>3120</v>
       </c>
-      <c r="V7" s="3">
+      <c r="V7" s="1">
         <v>62156.25</v>
       </c>
-      <c r="W7" s="3">
+      <c r="W7" s="1">
         <v>65.441176470588204</v>
       </c>
-      <c r="X7" s="3">
+      <c r="X7" s="1">
         <v>248.81372549019599</v>
       </c>
       <c r="Y7" s="1">
@@ -1867,7 +1852,7 @@
       <c r="AA7" s="1">
         <v>0</v>
       </c>
-      <c r="AB7" s="2">
+      <c r="AB7" s="1">
         <v>18.434948822921999</v>
       </c>
       <c r="AC7" s="1">
@@ -1885,17 +1870,15 @@
       <c r="AG7" s="1">
         <v>302</v>
       </c>
-      <c r="AH7" s="3">
+      <c r="AH7" s="1">
         <v>103.043783152882</v>
       </c>
-      <c r="AI7" s="3">
+      <c r="AI7" s="1">
         <v>6429.9320687398904</v>
       </c>
-      <c r="AJ7" s="1">
-        <v>2</v>
-      </c>
+      <c r="AJ7" s="1"/>
       <c r="AK7" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AL7" s="1">
         <v>0</v>
@@ -1911,62 +1894,60 @@
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="1">
         <v>75</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="1">
         <v>198.033114398283</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="1">
         <v>252</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="1">
         <v>93.75</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="1">
         <v>197.064466428911</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="1">
         <v>258.25</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="1">
         <v>84.375</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="1">
         <v>197.40314050704299</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="1">
         <v>255.125</v>
       </c>
-      <c r="K8" s="4">
-        <v>226.38039322298599</v>
-      </c>
-      <c r="L8" s="4">
+      <c r="K8" s="1"/>
+      <c r="L8" s="1">
         <v>18.75</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8" s="1">
         <v>-2.9559201572884599</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8" s="1">
         <v>18.7749800494549</v>
       </c>
       <c r="O8" s="1">
         <v>0</v>
       </c>
-      <c r="P8" s="3">
-        <v>29.596859492956401</v>
-      </c>
-      <c r="Q8" s="3">
-        <v>0</v>
-      </c>
-      <c r="R8" s="3">
-        <v>28.125</v>
-      </c>
-      <c r="S8" s="3">
-        <v>134175.72595563001</v>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0</v>
       </c>
       <c r="T8" s="1">
         <v>3120</v>
@@ -1974,13 +1955,13 @@
       <c r="U8" s="1">
         <v>2730</v>
       </c>
-      <c r="V8" s="3">
+      <c r="V8" s="1">
         <v>54843.75</v>
       </c>
-      <c r="W8" s="3">
+      <c r="W8" s="1">
         <v>84.1666666666666</v>
       </c>
-      <c r="X8" s="3">
+      <c r="X8" s="1">
         <v>255.055555555555</v>
       </c>
       <c r="Y8" s="1">
@@ -1992,7 +1973,7 @@
       <c r="AA8" s="1">
         <v>0</v>
       </c>
-      <c r="AB8" s="2">
+      <c r="AB8" s="1">
         <v>18.434948822921999</v>
       </c>
       <c r="AC8" s="1">
@@ -2010,17 +1991,15 @@
       <c r="AG8" s="1">
         <v>302</v>
       </c>
-      <c r="AH8" s="3">
+      <c r="AH8" s="1">
         <v>104.596859492956</v>
       </c>
-      <c r="AI8" s="3">
+      <c r="AI8" s="1">
         <v>6526.84403236048</v>
       </c>
-      <c r="AJ8" s="1">
-        <v>2</v>
-      </c>
+      <c r="AJ8" s="1"/>
       <c r="AK8" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AL8" s="1">
         <v>0</v>
@@ -2036,62 +2015,60 @@
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="1">
         <v>93.75</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="1">
         <v>197.064466428911</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="1">
         <v>258.25</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="1">
         <v>112.5</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="1">
         <v>197.25794808120801</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="1">
         <v>264.5</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="1">
         <v>103.125</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="1">
         <v>197.016115321293</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="1">
         <v>261.375</v>
       </c>
-      <c r="K9" s="4">
-        <v>229.32463842098301</v>
-      </c>
-      <c r="L9" s="4">
+      <c r="K9" s="1"/>
+      <c r="L9" s="1">
         <v>18.75</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9" s="1">
         <v>0.59093229529258096</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="1">
         <v>18.750997288271599</v>
       </c>
       <c r="O9" s="1">
         <v>0</v>
       </c>
-      <c r="P9" s="3">
-        <v>29.9838846787069</v>
-      </c>
-      <c r="Q9" s="3">
-        <v>0</v>
-      </c>
-      <c r="R9" s="3">
-        <v>34.375</v>
-      </c>
-      <c r="S9" s="3">
-        <v>149716.74029026699</v>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0</v>
       </c>
       <c r="T9" s="1">
         <v>2730</v>
@@ -2099,13 +2076,13 @@
       <c r="U9" s="1">
         <v>2340</v>
       </c>
-      <c r="V9" s="3">
+      <c r="V9" s="1">
         <v>47531.25</v>
       </c>
-      <c r="W9" s="3">
+      <c r="W9" s="1">
         <v>102.884615384615</v>
       </c>
-      <c r="X9" s="3">
+      <c r="X9" s="1">
         <v>261.29487179487103</v>
       </c>
       <c r="Y9" s="1">
@@ -2117,7 +2094,7 @@
       <c r="AA9" s="1">
         <v>0</v>
       </c>
-      <c r="AB9" s="2">
+      <c r="AB9" s="1">
         <v>18.434948822921999</v>
       </c>
       <c r="AC9" s="1">
@@ -2135,17 +2112,15 @@
       <c r="AG9" s="1">
         <v>302</v>
       </c>
-      <c r="AH9" s="3">
+      <c r="AH9" s="1">
         <v>104.983884678706</v>
       </c>
-      <c r="AI9" s="3">
+      <c r="AI9" s="1">
         <v>6550.9944039513102</v>
       </c>
-      <c r="AJ9" s="1">
-        <v>2</v>
-      </c>
+      <c r="AJ9" s="1"/>
       <c r="AK9" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AL9" s="1">
         <v>0</v>
@@ -2161,62 +2136,60 @@
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="1">
         <v>112.5</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="1">
         <v>197.25794808120801</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="1">
         <v>264.5</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="1">
         <v>131.25</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="1">
         <v>198.615797527474</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="1">
         <v>270.75</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="1">
         <v>121.875</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="1">
         <v>197.79066133721099</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="1">
         <v>267.625</v>
       </c>
-      <c r="K10" s="4">
-        <v>232.84468301247699</v>
-      </c>
-      <c r="L10" s="4">
+      <c r="K10" s="1"/>
+      <c r="L10" s="1">
         <v>18.75</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="1">
         <v>4.1400544371676897</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10" s="1">
         <v>18.799055069424998</v>
       </c>
       <c r="O10" s="1">
         <v>0</v>
       </c>
-      <c r="P10" s="3">
-        <v>29.2093386627885</v>
-      </c>
-      <c r="Q10" s="3">
-        <v>0</v>
-      </c>
-      <c r="R10" s="3">
-        <v>40.625</v>
-      </c>
-      <c r="S10" s="3">
-        <v>162578.88104105601</v>
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0</v>
       </c>
       <c r="T10" s="1">
         <v>2340</v>
@@ -2224,13 +2197,13 @@
       <c r="U10" s="1">
         <v>1950</v>
       </c>
-      <c r="V10" s="3">
+      <c r="V10" s="1">
         <v>40218.75</v>
       </c>
-      <c r="W10" s="3">
+      <c r="W10" s="1">
         <v>121.59090909090899</v>
       </c>
-      <c r="X10" s="3">
+      <c r="X10" s="1">
         <v>267.530303030303</v>
       </c>
       <c r="Y10" s="1">
@@ -2242,7 +2215,7 @@
       <c r="AA10" s="1">
         <v>0</v>
       </c>
-      <c r="AB10" s="2">
+      <c r="AB10" s="1">
         <v>18.434948822921999</v>
       </c>
       <c r="AC10" s="1">
@@ -2260,17 +2233,15 @@
       <c r="AG10" s="1">
         <v>302</v>
       </c>
-      <c r="AH10" s="3">
+      <c r="AH10" s="1">
         <v>104.209338662788</v>
       </c>
-      <c r="AI10" s="3">
+      <c r="AI10" s="1">
         <v>6502.6627325580002</v>
       </c>
-      <c r="AJ10" s="1">
-        <v>2</v>
-      </c>
+      <c r="AJ10" s="1"/>
       <c r="AK10" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AL10" s="1">
         <v>0</v>
@@ -2286,62 +2257,60 @@
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="1">
         <v>131.25</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="1">
         <v>198.615797527474</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="1">
         <v>270.75</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="1">
         <v>150</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="1">
         <v>201.15388575388801</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="1">
         <v>277</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="1">
         <v>140.625</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="1">
         <v>199.73576740643901</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="1">
         <v>273.875</v>
       </c>
-      <c r="K11" s="4">
-        <v>236.94410378987399</v>
-      </c>
-      <c r="L11" s="4">
+      <c r="K11" s="1"/>
+      <c r="L11" s="1">
         <v>18.75</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="1">
         <v>7.7051875121780897</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11" s="1">
         <v>18.920834995842199</v>
       </c>
       <c r="O11" s="1">
         <v>0</v>
       </c>
-      <c r="P11" s="3">
-        <v>27.264232593560799</v>
-      </c>
-      <c r="Q11" s="3">
-        <v>0</v>
-      </c>
-      <c r="R11" s="3">
-        <v>46.875</v>
-      </c>
-      <c r="S11" s="3">
-        <v>172741.417668899</v>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0</v>
       </c>
       <c r="T11" s="1">
         <v>1950</v>
@@ -2349,13 +2318,13 @@
       <c r="U11" s="1">
         <v>1560</v>
       </c>
-      <c r="V11" s="3">
+      <c r="V11" s="1">
         <v>32906.25</v>
       </c>
-      <c r="W11" s="3">
+      <c r="W11" s="1">
         <v>140.277777777777</v>
       </c>
-      <c r="X11" s="3">
+      <c r="X11" s="1">
         <v>273.75925925925901</v>
       </c>
       <c r="Y11" s="1">
@@ -2367,7 +2336,7 @@
       <c r="AA11" s="1">
         <v>0</v>
       </c>
-      <c r="AB11" s="2">
+      <c r="AB11" s="1">
         <v>18.434948822921999</v>
       </c>
       <c r="AC11" s="1">
@@ -2385,17 +2354,15 @@
       <c r="AG11" s="1">
         <v>302</v>
       </c>
-      <c r="AH11" s="3">
+      <c r="AH11" s="1">
         <v>102.26423259356</v>
       </c>
-      <c r="AI11" s="3">
+      <c r="AI11" s="1">
         <v>6381.2881138381899</v>
       </c>
-      <c r="AJ11" s="1">
-        <v>2</v>
-      </c>
+      <c r="AJ11" s="1"/>
       <c r="AK11" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AL11" s="1">
         <v>0</v>
@@ -2411,62 +2378,60 @@
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="1">
         <v>150</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="1">
         <v>201.15388575388801</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="1">
         <v>277</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="1">
         <v>168.75</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="1">
         <v>204.902664363095</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="1">
         <v>283.25</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="1">
         <v>159.375</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="1">
         <v>202.87442154031899</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="1">
         <v>280.125</v>
       </c>
-      <c r="K12" s="4">
-        <v>241.633106051646</v>
-      </c>
-      <c r="L12" s="4">
+      <c r="K12" s="1"/>
+      <c r="L12" s="1">
         <v>18.75</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="1">
         <v>11.300639884232901</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12" s="1">
         <v>19.120703204280201</v>
       </c>
       <c r="O12" s="1">
         <v>0</v>
       </c>
-      <c r="P12" s="3">
-        <v>24.125578459680899</v>
-      </c>
-      <c r="Q12" s="3">
-        <v>0</v>
-      </c>
-      <c r="R12" s="3">
-        <v>53.125</v>
-      </c>
-      <c r="S12" s="3">
-        <v>180151.334072639</v>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0</v>
       </c>
       <c r="T12" s="1">
         <v>1560</v>
@@ -2474,13 +2439,13 @@
       <c r="U12" s="1">
         <v>1169.99999999999</v>
       </c>
-      <c r="V12" s="3">
+      <c r="V12" s="1">
         <v>25593.75</v>
       </c>
-      <c r="W12" s="3">
+      <c r="W12" s="1">
         <v>158.92857142857099</v>
       </c>
-      <c r="X12" s="3">
+      <c r="X12" s="1">
         <v>279.97619047619003</v>
       </c>
       <c r="Y12" s="1">
@@ -2492,7 +2457,7 @@
       <c r="AA12" s="1">
         <v>0</v>
       </c>
-      <c r="AB12" s="2">
+      <c r="AB12" s="1">
         <v>18.434948822921999</v>
       </c>
       <c r="AC12" s="1">
@@ -2510,17 +2475,15 @@
       <c r="AG12" s="1">
         <v>302</v>
       </c>
-      <c r="AH12" s="3">
+      <c r="AH12" s="1">
         <v>99.125578459680895</v>
       </c>
-      <c r="AI12" s="3">
+      <c r="AI12" s="1">
         <v>6185.4360958840898</v>
       </c>
-      <c r="AJ12" s="1">
-        <v>2</v>
-      </c>
+      <c r="AJ12" s="1"/>
       <c r="AK12" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AL12" s="1">
         <v>0</v>
@@ -2536,62 +2499,60 @@
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="1">
         <v>168.75</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="1">
         <v>204.902664363095</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="1">
         <v>283.25</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="1">
         <v>187.5</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="1">
         <v>209.909065981027</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="1">
         <v>289.5</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="1">
         <v>178.125</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="1">
         <v>207.24500964970699</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="1">
         <v>286.375</v>
       </c>
-      <c r="K13" s="4">
-        <v>246.92906528456501</v>
-      </c>
-      <c r="L13" s="4">
+      <c r="K13" s="1"/>
+      <c r="L13" s="1">
         <v>18.75</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13" s="1">
         <v>14.9418321374851</v>
       </c>
-      <c r="N13" s="4">
+      <c r="N13" s="1">
         <v>19.406159373882101</v>
       </c>
       <c r="O13" s="1">
         <v>0</v>
       </c>
-      <c r="P13" s="3">
-        <v>19.754990350292701</v>
-      </c>
-      <c r="Q13" s="3">
-        <v>0</v>
-      </c>
-      <c r="R13" s="3">
-        <v>59.375</v>
-      </c>
-      <c r="S13" s="3">
-        <v>184720.102745362</v>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0</v>
       </c>
       <c r="T13" s="1">
         <v>1169.99999999999</v>
@@ -2599,13 +2560,13 @@
       <c r="U13" s="1">
         <v>779.99999999999898</v>
       </c>
-      <c r="V13" s="3">
+      <c r="V13" s="1">
         <v>18281.249999999902</v>
       </c>
-      <c r="W13" s="3">
+      <c r="W13" s="1">
         <v>177.5</v>
       </c>
-      <c r="X13" s="3">
+      <c r="X13" s="1">
         <v>286.166666666666</v>
       </c>
       <c r="Y13" s="1">
@@ -2617,7 +2578,7 @@
       <c r="AA13" s="1">
         <v>0</v>
       </c>
-      <c r="AB13" s="2">
+      <c r="AB13" s="1">
         <v>18.434948822921999</v>
       </c>
       <c r="AC13" s="1">
@@ -2635,17 +2596,15 @@
       <c r="AG13" s="1">
         <v>302</v>
       </c>
-      <c r="AH13" s="3">
+      <c r="AH13" s="1">
         <v>94.754990350292701</v>
       </c>
-      <c r="AI13" s="3">
+      <c r="AI13" s="1">
         <v>5912.7113978582602</v>
       </c>
-      <c r="AJ13" s="1">
-        <v>2</v>
-      </c>
+      <c r="AJ13" s="1"/>
       <c r="AK13" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AL13" s="1">
         <v>0</v>
@@ -2661,62 +2620,60 @@
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="1">
         <v>187.5</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="1">
         <v>209.909065981027</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="1">
         <v>289.5</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="1">
         <v>206.25</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="1">
         <v>216.23964776593601</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="1">
         <v>295.75</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="1">
         <v>196.875</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="1">
         <v>212.90378899226101</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="1">
         <v>292.625</v>
       </c>
-      <c r="K14" s="4">
-        <v>252.85748775048199</v>
-      </c>
-      <c r="L14" s="4">
+      <c r="K14" s="1"/>
+      <c r="L14" s="1">
         <v>18.75</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14" s="1">
         <v>18.645960602344999</v>
       </c>
-      <c r="N14" s="4">
+      <c r="N14" s="1">
         <v>19.788662415468998</v>
       </c>
       <c r="O14" s="1">
         <v>0</v>
       </c>
-      <c r="P14" s="3">
-        <v>14.096211007738599</v>
-      </c>
-      <c r="Q14" s="3">
-        <v>0</v>
-      </c>
-      <c r="R14" s="3">
-        <v>65.625</v>
-      </c>
-      <c r="S14" s="3">
-        <v>186317.98038659699</v>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>0</v>
+      </c>
+      <c r="R14" s="1">
+        <v>0</v>
+      </c>
+      <c r="S14" s="1">
+        <v>0</v>
       </c>
       <c r="T14" s="1">
         <v>779.99999999999898</v>
@@ -2724,13 +2681,13 @@
       <c r="U14" s="1">
         <v>389.99999999999898</v>
       </c>
-      <c r="V14" s="3">
+      <c r="V14" s="1">
         <v>10968.7499999999</v>
       </c>
-      <c r="W14" s="3">
+      <c r="W14" s="1">
         <v>195.833333333333</v>
       </c>
-      <c r="X14" s="3">
+      <c r="X14" s="1">
         <v>292.27777777777698</v>
       </c>
       <c r="Y14" s="1">
@@ -2742,7 +2699,7 @@
       <c r="AA14" s="1">
         <v>0</v>
       </c>
-      <c r="AB14" s="2">
+      <c r="AB14" s="1">
         <v>18.434948822921999</v>
       </c>
       <c r="AC14" s="1">
@@ -2760,17 +2717,15 @@
       <c r="AG14" s="1">
         <v>302</v>
       </c>
-      <c r="AH14" s="3">
+      <c r="AH14" s="1">
         <v>89.096211007738603</v>
       </c>
-      <c r="AI14" s="3">
+      <c r="AI14" s="1">
         <v>5559.6035668828899</v>
       </c>
-      <c r="AJ14" s="1">
-        <v>2</v>
-      </c>
+      <c r="AJ14" s="1"/>
       <c r="AK14" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AL14" s="1">
         <v>0</v>
@@ -2786,62 +2741,60 @@
       </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="1">
         <v>206.25</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="1">
         <v>216.23964776593601</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="1">
         <v>295.75</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="1">
         <v>225</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="1">
         <v>223.98550762686301</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="1">
         <v>302</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="1">
         <v>215.625</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="1">
         <v>219.92883158918301</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="1">
         <v>298.875</v>
       </c>
-      <c r="K15" s="4">
-        <v>259.45349216874399</v>
-      </c>
-      <c r="L15" s="4">
+      <c r="K15" s="1"/>
+      <c r="L15" s="1">
         <v>18.75</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15" s="1">
         <v>22.4328665373211</v>
       </c>
-      <c r="N15" s="4">
+      <c r="N15" s="1">
         <v>20.285022670689401</v>
       </c>
       <c r="O15" s="1">
         <v>0</v>
       </c>
-      <c r="P15" s="3">
-        <v>7.0711684108165898</v>
-      </c>
-      <c r="Q15" s="3">
-        <v>0</v>
-      </c>
-      <c r="R15" s="3">
-        <v>71.875</v>
-      </c>
-      <c r="S15" s="3">
-        <v>184764.91339744499</v>
+      <c r="P15" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>0</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0</v>
       </c>
       <c r="T15" s="1">
         <v>389.99999999999898</v>
@@ -2849,13 +2802,13 @@
       <c r="U15" s="1">
         <v>0</v>
       </c>
-      <c r="V15" s="3">
+      <c r="V15" s="1">
         <v>3656.24999999999</v>
       </c>
-      <c r="W15" s="3">
+      <c r="W15" s="1">
         <v>212.5</v>
       </c>
-      <c r="X15" s="3">
+      <c r="X15" s="1">
         <v>297.83333333333297</v>
       </c>
       <c r="Y15" s="1">
@@ -2867,7 +2820,7 @@
       <c r="AA15" s="1">
         <v>0</v>
       </c>
-      <c r="AB15" s="2">
+      <c r="AB15" s="1">
         <v>18.434948822921999</v>
       </c>
       <c r="AC15" s="1">
@@ -2885,17 +2838,15 @@
       <c r="AG15" s="1">
         <v>302</v>
       </c>
-      <c r="AH15" s="3">
+      <c r="AH15" s="1">
         <v>82.071168410816597</v>
       </c>
-      <c r="AI15" s="3">
+      <c r="AI15" s="1">
         <v>5121.2409088349496</v>
       </c>
-      <c r="AJ15" s="1">
-        <v>2</v>
-      </c>
+      <c r="AJ15" s="1"/>
       <c r="AK15" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AL15" s="1">
         <v>0</v>
@@ -2911,62 +2862,60 @@
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="1">
         <v>225</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="1">
         <v>223.98550762686301</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="1">
         <v>302</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="1">
         <v>240</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="1">
         <v>231.282676405111</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="1">
         <v>307</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="1">
         <v>232.5</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="1">
         <v>227.506422094024</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="1">
         <v>304.5</v>
       </c>
-      <c r="K16" s="4">
-        <v>266.00321104701197</v>
-      </c>
-      <c r="L16" s="4">
+      <c r="K16" s="1"/>
+      <c r="L16" s="1">
         <v>15</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16" s="1">
         <v>25.931337514528501</v>
       </c>
-      <c r="N16" s="4">
+      <c r="N16" s="1">
         <v>16.679292171393701</v>
       </c>
       <c r="O16" s="1">
         <v>0</v>
       </c>
-      <c r="P16" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="3">
-        <v>0</v>
-      </c>
-      <c r="R16" s="3">
-        <v>76.993577905975599</v>
-      </c>
-      <c r="S16" s="3">
-        <v>144362.958573704</v>
+      <c r="P16" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0</v>
       </c>
       <c r="T16" s="1">
         <v>0</v>
@@ -2974,13 +2923,13 @@
       <c r="U16" s="1">
         <v>0</v>
       </c>
-      <c r="V16" s="3">
-        <v>0</v>
-      </c>
-      <c r="W16" s="3">
+      <c r="V16" s="1">
+        <v>0</v>
+      </c>
+      <c r="W16" s="1">
         <v>232.5</v>
       </c>
-      <c r="X16" s="3">
+      <c r="X16" s="1">
         <v>304.5</v>
       </c>
       <c r="Y16" s="1">
@@ -2992,7 +2941,7 @@
       <c r="AA16" s="1">
         <v>0</v>
       </c>
-      <c r="AB16" s="2">
+      <c r="AB16" s="1">
         <v>18.434948822921999</v>
       </c>
       <c r="AC16" s="1">
@@ -3010,17 +2959,15 @@
       <c r="AG16" s="1">
         <v>302</v>
       </c>
-      <c r="AH16" s="3">
+      <c r="AH16" s="1">
         <v>74.493577905975599</v>
       </c>
-      <c r="AI16" s="3">
+      <c r="AI16" s="1">
         <v>4648.3992613328701</v>
       </c>
-      <c r="AJ16" s="1">
-        <v>4</v>
-      </c>
+      <c r="AJ16" s="1"/>
       <c r="AK16" s="1">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="AL16" s="1">
         <v>0</v>
@@ -3036,61 +2983,61 @@
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="1">
         <v>240</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="1">
         <v>231.282676405111</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="1">
         <v>307</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="1">
         <v>255</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="1">
         <v>239.646394301903</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="1">
         <v>312</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="1">
         <v>247.5</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="1">
         <v>235.32519953724301</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="1">
         <v>309.5</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="1">
         <v>272.48564735641099</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="1">
         <v>15</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17" s="1">
         <v>29.1303843971112</v>
       </c>
-      <c r="N17" s="4">
+      <c r="N17" s="1">
         <v>17.172016350116699</v>
       </c>
       <c r="O17" s="1">
-        <v>0</v>
-      </c>
-      <c r="P17" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="3">
+        <v>67.5</v>
+      </c>
+      <c r="P17" s="1">
         <v>6.6748004627565303</v>
       </c>
-      <c r="R17" s="3">
-        <v>67.5</v>
-      </c>
-      <c r="S17" s="3">
+      <c r="Q17" s="1">
+        <v>0</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0</v>
+      </c>
+      <c r="S17" s="1">
         <v>138777.38484684401</v>
       </c>
       <c r="T17" s="1">
@@ -3099,13 +3046,13 @@
       <c r="U17" s="1">
         <v>0</v>
       </c>
-      <c r="V17" s="3">
-        <v>0</v>
-      </c>
-      <c r="W17" s="3">
+      <c r="V17" s="1">
+        <v>0</v>
+      </c>
+      <c r="W17" s="1">
         <v>247.5</v>
       </c>
-      <c r="X17" s="3">
+      <c r="X17" s="1">
         <v>309.5</v>
       </c>
       <c r="Y17" s="1">
@@ -3117,7 +3064,7 @@
       <c r="AA17" s="1">
         <v>0</v>
       </c>
-      <c r="AB17" s="2">
+      <c r="AB17" s="1">
         <v>18.434948822921999</v>
       </c>
       <c r="AC17" s="1">
@@ -3135,20 +3082,20 @@
       <c r="AG17" s="1">
         <v>302</v>
       </c>
-      <c r="AH17" s="3">
+      <c r="AH17" s="1">
         <v>66.674800462756494</v>
       </c>
-      <c r="AI17" s="3">
+      <c r="AI17" s="1">
         <v>4160.5075488760003</v>
       </c>
       <c r="AJ17" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AK17" s="1">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="AL17" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AM17" s="1">
         <v>303</v>
@@ -3161,61 +3108,61 @@
       </c>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="1">
         <v>255</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="1">
         <v>239.646394301903</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="1">
         <v>312</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="1">
         <v>270</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="1">
         <v>249.18333388707899</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="1">
         <v>317</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="1">
         <v>262.5</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="1">
         <v>244.26038633015801</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="1">
         <v>314.5</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="1">
         <v>279.583533936648</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="1">
         <v>15</v>
       </c>
-      <c r="M18" s="4">
+      <c r="M18" s="1">
         <v>32.432363702317502</v>
       </c>
-      <c r="N18" s="4">
+      <c r="N18" s="1">
         <v>17.771982745196201</v>
       </c>
       <c r="O18" s="1">
-        <v>0</v>
-      </c>
-      <c r="P18" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="3">
+        <v>42.5</v>
+      </c>
+      <c r="P18" s="1">
         <v>27.739613669841901</v>
       </c>
-      <c r="R18" s="3">
-        <v>42.5</v>
-      </c>
-      <c r="S18" s="3">
+      <c r="Q18" s="1">
+        <v>0</v>
+      </c>
+      <c r="R18" s="1">
+        <v>0</v>
+      </c>
+      <c r="S18" s="1">
         <v>130450.99301581</v>
       </c>
       <c r="T18" s="1">
@@ -3224,13 +3171,13 @@
       <c r="U18" s="1">
         <v>0</v>
       </c>
-      <c r="V18" s="3">
-        <v>0</v>
-      </c>
-      <c r="W18" s="3">
+      <c r="V18" s="1">
+        <v>0</v>
+      </c>
+      <c r="W18" s="1">
         <v>262.5</v>
       </c>
-      <c r="X18" s="3">
+      <c r="X18" s="1">
         <v>314.5</v>
       </c>
       <c r="Y18" s="1">
@@ -3242,7 +3189,7 @@
       <c r="AA18" s="1">
         <v>0</v>
       </c>
-      <c r="AB18" s="2">
+      <c r="AB18" s="1">
         <v>18.434948822921999</v>
       </c>
       <c r="AC18" s="1">
@@ -3260,20 +3207,20 @@
       <c r="AG18" s="1">
         <v>302</v>
       </c>
-      <c r="AH18" s="3">
+      <c r="AH18" s="1">
         <v>57.739613669841901</v>
       </c>
-      <c r="AI18" s="3">
+      <c r="AI18" s="1">
         <v>3602.95189299813</v>
       </c>
       <c r="AJ18" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AK18" s="1">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="AL18" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AM18" s="1">
         <v>303</v>
@@ -3286,61 +3233,61 @@
       </c>
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="1">
         <v>270</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="1">
         <v>249.18333388707899</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="1">
         <v>317</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="1">
         <v>280</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="1">
         <v>256.26038483660398</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="1">
         <v>317</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="1">
         <v>275</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="1">
         <v>252.64600266015501</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19" s="1">
         <v>317</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19" s="1">
         <v>284.99119604050202</v>
       </c>
-      <c r="L19" s="4">
+      <c r="L19" s="1">
         <v>10</v>
       </c>
-      <c r="M19" s="4">
+      <c r="M19" s="1">
         <v>35.278950920886103</v>
       </c>
-      <c r="N19" s="4">
+      <c r="N19" s="1">
         <v>12.2496504355149</v>
       </c>
       <c r="O19" s="1">
-        <v>0</v>
-      </c>
-      <c r="P19" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="3">
+        <v>20</v>
+      </c>
+      <c r="P19" s="1">
         <v>44.353997339844902</v>
       </c>
-      <c r="R19" s="3">
-        <v>20</v>
-      </c>
-      <c r="S19" s="3">
+      <c r="Q19" s="1">
+        <v>0</v>
+      </c>
+      <c r="R19" s="1">
+        <v>0</v>
+      </c>
+      <c r="S19" s="1">
         <v>79111.876754610697</v>
       </c>
       <c r="T19" s="1">
@@ -3349,13 +3296,13 @@
       <c r="U19" s="1">
         <v>0</v>
       </c>
-      <c r="V19" s="3">
-        <v>0</v>
-      </c>
-      <c r="W19" s="3">
+      <c r="V19" s="1">
+        <v>0</v>
+      </c>
+      <c r="W19" s="1">
         <v>275</v>
       </c>
-      <c r="X19" s="3">
+      <c r="X19" s="1">
         <v>317</v>
       </c>
       <c r="Y19" s="1">
@@ -3367,7 +3314,7 @@
       <c r="AA19" s="1">
         <v>0</v>
       </c>
-      <c r="AB19" s="2">
+      <c r="AB19" s="1">
         <v>0</v>
       </c>
       <c r="AC19" s="1">
@@ -3385,20 +3332,20 @@
       <c r="AG19" s="1">
         <v>302</v>
       </c>
-      <c r="AH19" s="3">
+      <c r="AH19" s="1">
         <v>49.353997339844902</v>
       </c>
-      <c r="AI19" s="3">
+      <c r="AI19" s="1">
         <v>3079.68943400632</v>
       </c>
       <c r="AJ19" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AK19" s="1">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="AL19" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AM19" s="1">
         <v>303</v>
@@ -3411,61 +3358,61 @@
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="1">
         <v>280</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="1">
         <v>256.26038483660398</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="1">
         <v>317</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="1">
         <v>295</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="1">
         <v>268.08622291894699</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="1">
         <v>317</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="1">
         <v>287.5</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="1">
         <v>261.98161835690001</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="1">
         <v>317</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="1">
         <v>289.59096513080402</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="1">
         <v>15</v>
       </c>
-      <c r="M20" s="4">
+      <c r="M20" s="1">
         <v>38.229423600919397</v>
       </c>
-      <c r="N20" s="4">
+      <c r="N20" s="1">
         <v>19.095163873953702</v>
       </c>
       <c r="O20" s="1">
-        <v>0</v>
-      </c>
-      <c r="P20" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="3">
+        <v>10</v>
+      </c>
+      <c r="P20" s="1">
         <v>45.018381643099097</v>
       </c>
-      <c r="R20" s="3">
-        <v>10</v>
-      </c>
-      <c r="S20" s="3">
+      <c r="Q20" s="1">
+        <v>0</v>
+      </c>
+      <c r="R20" s="1">
+        <v>0</v>
+      </c>
+      <c r="S20" s="1">
         <v>101133.638406871</v>
       </c>
       <c r="T20" s="1">
@@ -3474,13 +3421,13 @@
       <c r="U20" s="1">
         <v>0</v>
       </c>
-      <c r="V20" s="3">
-        <v>0</v>
-      </c>
-      <c r="W20" s="3">
+      <c r="V20" s="1">
+        <v>0</v>
+      </c>
+      <c r="W20" s="1">
         <v>287.5</v>
       </c>
-      <c r="X20" s="3">
+      <c r="X20" s="1">
         <v>317</v>
       </c>
       <c r="Y20" s="1">
@@ -3492,7 +3439,7 @@
       <c r="AA20" s="1">
         <v>0</v>
       </c>
-      <c r="AB20" s="2">
+      <c r="AB20" s="1">
         <v>0</v>
       </c>
       <c r="AC20" s="1">
@@ -3510,20 +3457,20 @@
       <c r="AG20" s="1">
         <v>294.8</v>
       </c>
-      <c r="AH20" s="3">
+      <c r="AH20" s="1">
         <v>32.818381643099102</v>
       </c>
-      <c r="AI20" s="3">
+      <c r="AI20" s="1">
         <v>2047.86701452938</v>
       </c>
       <c r="AJ20" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AK20" s="1">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="AL20" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AM20" s="1">
         <v>303</v>
@@ -3536,61 +3483,61 @@
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="1">
         <v>295</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="1">
         <v>268.08622291894699</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="1">
         <v>317</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="1">
         <v>310</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="1">
         <v>281.57610020879099</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="1">
         <v>317</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="1">
         <v>302.5</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="1">
         <v>274.60534611486401</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="1">
         <v>317</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="1">
         <v>295.89608059397</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21" s="1">
         <v>15</v>
       </c>
-      <c r="M21" s="4">
+      <c r="M21" s="1">
         <v>41.9372896627372</v>
       </c>
-      <c r="N21" s="4">
+      <c r="N21" s="1">
         <v>20.164630905231</v>
       </c>
       <c r="O21" s="1">
-        <v>0</v>
-      </c>
-      <c r="P21" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="3">
+        <v>10</v>
+      </c>
+      <c r="P21" s="1">
         <v>32.394653885135398</v>
       </c>
-      <c r="R21" s="3">
-        <v>10</v>
-      </c>
-      <c r="S21" s="3">
+      <c r="Q21" s="1">
+        <v>0</v>
+      </c>
+      <c r="R21" s="1">
+        <v>0</v>
+      </c>
+      <c r="S21" s="1">
         <v>78032.216609797804</v>
       </c>
       <c r="T21" s="1">
@@ -3599,13 +3546,13 @@
       <c r="U21" s="1">
         <v>0</v>
       </c>
-      <c r="V21" s="3">
-        <v>0</v>
-      </c>
-      <c r="W21" s="3">
+      <c r="V21" s="1">
+        <v>0</v>
+      </c>
+      <c r="W21" s="1">
         <v>302.5</v>
       </c>
-      <c r="X21" s="3">
+      <c r="X21" s="1">
         <v>317</v>
       </c>
       <c r="Y21" s="1">
@@ -3617,7 +3564,7 @@
       <c r="AA21" s="1">
         <v>0</v>
       </c>
-      <c r="AB21" s="2">
+      <c r="AB21" s="1">
         <v>0</v>
       </c>
       <c r="AC21" s="1">
@@ -3635,20 +3582,20 @@
       <c r="AG21" s="1">
         <v>284</v>
       </c>
-      <c r="AH21" s="3">
+      <c r="AH21" s="1">
         <v>9.3946538851354209</v>
       </c>
-      <c r="AI21" s="3">
+      <c r="AI21" s="1">
         <v>586.22640243244996</v>
       </c>
       <c r="AJ21" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AK21" s="1">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="AL21" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AM21" s="1">
         <v>303</v>
@@ -3661,61 +3608,61 @@
       </c>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="1">
         <v>310</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="1">
         <v>281.57610020879099</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="1">
         <v>317</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="1">
         <v>320</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="1">
         <v>291.651733868505</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="1">
         <v>317</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="1">
         <v>315</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="1">
         <v>286.49590167867899</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="1">
         <v>317</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22" s="1">
         <v>301.83128363057</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22" s="1">
         <v>10</v>
       </c>
-      <c r="M22" s="4">
+      <c r="M22" s="1">
         <v>45.200017997556202</v>
       </c>
-      <c r="N22" s="4">
+      <c r="N22" s="1">
         <v>14.191765063025599</v>
       </c>
       <c r="O22" s="1">
-        <v>0</v>
-      </c>
-      <c r="P22" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="3">
+        <v>20</v>
+      </c>
+      <c r="P22" s="1">
         <v>10.5040983213202</v>
       </c>
-      <c r="R22" s="3">
-        <v>20</v>
-      </c>
-      <c r="S22" s="3">
+      <c r="Q22" s="1">
+        <v>0</v>
+      </c>
+      <c r="R22" s="1">
+        <v>0</v>
+      </c>
+      <c r="S22" s="1">
         <v>37814.999952010701</v>
       </c>
       <c r="T22" s="1">
@@ -3724,13 +3671,13 @@
       <c r="U22" s="1">
         <v>0</v>
       </c>
-      <c r="V22" s="3">
-        <v>0</v>
-      </c>
-      <c r="W22" s="3">
+      <c r="V22" s="1">
+        <v>0</v>
+      </c>
+      <c r="W22" s="1">
         <v>315</v>
       </c>
-      <c r="X22" s="3">
+      <c r="X22" s="1">
         <v>317</v>
       </c>
       <c r="Y22" s="1">
@@ -3742,7 +3689,7 @@
       <c r="AA22" s="1">
         <v>0</v>
       </c>
-      <c r="AB22" s="2">
+      <c r="AB22" s="1">
         <v>0</v>
       </c>
       <c r="AC22" s="1">
@@ -3760,20 +3707,20 @@
       <c r="AG22" s="1">
         <v>275</v>
       </c>
-      <c r="AH22" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI22" s="3">
+      <c r="AH22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI22" s="1">
         <v>0</v>
       </c>
       <c r="AJ22" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AK22" s="1">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="AL22" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AM22" s="1">
         <v>303</v>
@@ -3786,61 +3733,61 @@
       </c>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="1">
         <v>320</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="1">
         <v>291.651733868505</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="1">
         <v>317</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="1">
         <v>337.051583908027</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="1">
         <v>311.27918353637898</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="1">
         <v>311.31613869732399</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="1">
         <v>328.52579195401302</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="1">
         <v>301.04029952829399</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="1">
         <v>314.15806934866202</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="1">
         <v>307.59918443847801</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23" s="1">
         <v>17.051583908026998</v>
       </c>
-      <c r="M23" s="4">
+      <c r="M23" s="1">
         <v>48.956435837041397</v>
       </c>
-      <c r="N23" s="4">
+      <c r="N23" s="1">
         <v>25.968223316053301</v>
       </c>
       <c r="O23" s="1">
-        <v>0</v>
-      </c>
-      <c r="P23" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="3">
-        <v>0</v>
-      </c>
-      <c r="R23" s="3">
         <v>13.1177698203681</v>
       </c>
-      <c r="S23" s="3">
+      <c r="P23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>0</v>
+      </c>
+      <c r="R23" s="1">
+        <v>0</v>
+      </c>
+      <c r="S23" s="1">
         <v>27959.844097273901</v>
       </c>
       <c r="T23" s="1">
@@ -3849,13 +3796,13 @@
       <c r="U23" s="1">
         <v>0</v>
       </c>
-      <c r="V23" s="3">
-        <v>0</v>
-      </c>
-      <c r="W23" s="3">
+      <c r="V23" s="1">
+        <v>0</v>
+      </c>
+      <c r="W23" s="1">
         <v>328.52579195401302</v>
       </c>
-      <c r="X23" s="3">
+      <c r="X23" s="1">
         <v>314.15806934866202</v>
       </c>
       <c r="Y23" s="1">
@@ -3867,7 +3814,7 @@
       <c r="AA23" s="1">
         <v>0</v>
       </c>
-      <c r="AB23" s="2">
+      <c r="AB23" s="1">
         <v>-18.434948822921999</v>
       </c>
       <c r="AC23" s="1">
@@ -3885,14 +3832,14 @@
       <c r="AG23" s="1">
         <v>258.38937830208801</v>
       </c>
-      <c r="AH23" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI23" s="3">
+      <c r="AH23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI23" s="1">
         <v>0</v>
       </c>
       <c r="AJ23" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AK23" s="1">
         <v>34</v>

</xml_diff>